<commit_message>
Finalização e Alguns Resultados Obtidos
</commit_message>
<xml_diff>
--- a/pest/result_100it_10Kind.xlsx
+++ b/pest/result_100it_10Kind.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -2563,24 +2563,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73367936"/>
-        <c:axId val="73369472"/>
+        <c:axId val="75732096"/>
+        <c:axId val="75733632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73367936"/>
+        <c:axId val="75732096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73369472"/>
+        <c:crossAx val="75733632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73369472"/>
+        <c:axId val="75733632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,7 +2588,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73367936"/>
+        <c:crossAx val="75732096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2601,7 +2601,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5393,7 +5393,7 @@
         <v>7</v>
       </c>
       <c r="B103">
-        <f t="shared" ref="A103:F103" si="2">MEDIAN(B2:B102)</f>
+        <f t="shared" ref="B103:F103" si="2">MEDIAN(B2:B102)</f>
         <v>486</v>
       </c>
       <c r="C103">

</xml_diff>